<commit_message>
Market Basket Analysis using Apriori & PySpark
</commit_message>
<xml_diff>
--- a/Course_4-Big_Data_Processing_using_Apache_Spark/Market_Basket_Analysis_Assignment/MLC_C3_Assignment/c3_assignment_solution_file.xlsx
+++ b/Course_4-Big_Data_Processing_using_Apache_Spark/Market_Basket_Analysis_Assignment/MLC_C3_Assignment/c3_assignment_solution_file.xlsx
@@ -296,7 +296,7 @@
     <t>Discount %</t>
   </si>
   <si>
-    <t>{burgers} -&gt; {pancakes}</t>
+    <t>{burgers} -&gt; {frozen vegetables}</t>
   </si>
   <si>
     <t>[1.893770166294366]</t>
@@ -412,7 +412,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border/>
     <border>
       <left style="medium">
@@ -520,11 +520,50 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -563,6 +602,15 @@
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
   </cellXfs>
@@ -33592,41 +33640,41 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="6.86"/>
     <col customWidth="1" min="2" max="2" width="35.57"/>
-    <col customWidth="1" min="3" max="3" width="42.29"/>
+    <col customWidth="1" min="3" max="3" width="36.29"/>
     <col customWidth="1" min="4" max="4" width="17.71"/>
-    <col customWidth="1" min="5" max="5" width="19.14"/>
-    <col customWidth="1" min="6" max="6" width="38.71"/>
+    <col customWidth="1" min="5" max="5" width="26.43"/>
+    <col customWidth="1" min="6" max="6" width="42.86"/>
     <col customWidth="1" min="7" max="7" width="24.43"/>
     <col customWidth="1" min="8" max="9" width="18.14"/>
     <col customWidth="1" min="10" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="18" t="s">
         <v>67</v>
       </c>
       <c r="J1" s="8"/>
@@ -33648,10 +33696,10 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2">
-      <c r="A2" s="10">
+      <c r="A2" s="13">
         <v>1.0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -33661,7 +33709,7 @@
         <v>0.120795107033639</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>93</v>
@@ -33672,8 +33720,8 @@
       <c r="H2" s="11">
         <v>180.0</v>
       </c>
-      <c r="I2" s="11">
-        <v>-4.46885083147183</v>
+      <c r="I2" s="19">
+        <v>180.351605273532</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
@@ -33694,7 +33742,7 @@
       <c r="Z2" s="12"/>
     </row>
     <row r="3">
-      <c r="A3" s="14">
+      <c r="A3" s="13">
         <v>2.0</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -33718,8 +33766,8 @@
       <c r="H3" s="11">
         <v>75.0</v>
       </c>
-      <c r="I3" s="11">
-        <v>0.539974503733376</v>
+      <c r="I3" s="19">
+        <v>75.5399745037334</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
@@ -33740,7 +33788,7 @@
       <c r="Z3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="14">
+      <c r="A4" s="13">
         <v>3.0</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -33764,8 +33812,8 @@
       <c r="H4" s="11">
         <v>15.0</v>
       </c>
-      <c r="I4" s="11">
-        <v>0.539974503733381</v>
+      <c r="I4" s="19">
+        <v>15.5399745037334</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -33786,7 +33834,7 @@
       <c r="Z4" s="12"/>
     </row>
     <row r="5">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <v>4.0</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -33810,8 +33858,8 @@
       <c r="H5" s="11">
         <v>180.0</v>
       </c>
-      <c r="I5" s="11">
-        <v>1.36867387997194</v>
+      <c r="I5" s="19">
+        <v>181.368673879972</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
@@ -33832,7 +33880,7 @@
       <c r="Z5" s="12"/>
     </row>
     <row r="6">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
         <v>5.0</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -33856,8 +33904,8 @@
       <c r="H6" s="11">
         <v>170.0</v>
       </c>
-      <c r="I6" s="11">
-        <v>0.626101321585907</v>
+      <c r="I6" s="19">
+        <v>170.626101321586</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -33878,7 +33926,7 @@
       <c r="Z6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="14">
+      <c r="A7" s="13">
         <v>6.0</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -33902,8 +33950,8 @@
       <c r="H7" s="11">
         <v>65.0</v>
       </c>
-      <c r="I7" s="11">
-        <v>-0.0347591359768273</v>
+      <c r="I7" s="19">
+        <v>64.9652408640232</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
@@ -33924,7 +33972,7 @@
       <c r="Z7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>7.0</v>
       </c>
       <c r="B8" s="14" t="s">
@@ -33948,8 +33996,8 @@
       <c r="H8" s="11">
         <v>50.0</v>
       </c>
-      <c r="I8" s="11">
-        <v>-2.36707820978742</v>
+      <c r="I8" s="19">
+        <v>47.6329217902126</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -33970,7 +34018,7 @@
       <c r="Z8" s="12"/>
     </row>
     <row r="9">
-      <c r="A9" s="14">
+      <c r="A9" s="13">
         <v>8.0</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -33994,8 +34042,8 @@
       <c r="H9" s="11">
         <v>130.0</v>
       </c>
-      <c r="I9" s="11">
-        <v>-2.76040373955489</v>
+      <c r="I9" s="19">
+        <v>127.239596260445</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
@@ -34016,7 +34064,7 @@
       <c r="Z9" s="12"/>
     </row>
     <row r="10">
-      <c r="A10" s="14">
+      <c r="A10" s="13">
         <v>9.0</v>
       </c>
       <c r="B10" s="14" t="s">
@@ -34040,8 +34088,8 @@
       <c r="H10" s="11">
         <v>210.0</v>
       </c>
-      <c r="I10" s="11">
-        <v>-2.59727090142954</v>
+      <c r="I10" s="19">
+        <v>207.40272909857</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -34062,7 +34110,7 @@
       <c r="Z10" s="12"/>
     </row>
     <row r="11">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <v>10.0</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -34086,8 +34134,8 @@
       <c r="H11" s="11">
         <v>90.0</v>
       </c>
-      <c r="I11" s="11">
-        <v>0.80929700895409</v>
+      <c r="I11" s="19">
+        <v>90.8092970089541</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -34108,7 +34156,7 @@
       <c r="Z11" s="12"/>
     </row>
     <row r="12">
-      <c r="A12" s="14">
+      <c r="A12" s="13">
         <v>11.0</v>
       </c>
       <c r="B12" s="14" t="s">
@@ -34132,8 +34180,8 @@
       <c r="H12" s="11">
         <v>210.0</v>
       </c>
-      <c r="I12" s="11">
-        <v>-20.3878527020564</v>
+      <c r="I12" s="19">
+        <v>189.612147297944</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
@@ -34154,7 +34202,7 @@
       <c r="Z12" s="12"/>
     </row>
     <row r="13">
-      <c r="A13" s="14">
+      <c r="A13" s="13">
         <v>12.0</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -34178,8 +34226,8 @@
       <c r="H13" s="11">
         <v>280.0</v>
       </c>
-      <c r="I13" s="11">
-        <v>-0.0347591359768558</v>
+      <c r="I13" s="19">
+        <v>279.965240864023</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -34200,7 +34248,7 @@
       <c r="Z13" s="12"/>
     </row>
     <row r="14">
-      <c r="A14" s="14">
+      <c r="A14" s="13">
         <v>13.0</v>
       </c>
       <c r="B14" s="14" t="s">
@@ -34224,8 +34272,8 @@
       <c r="H14" s="11">
         <v>70.0</v>
       </c>
-      <c r="I14" s="11">
-        <v>1.96337869463466</v>
+      <c r="I14" s="19">
+        <v>71.9633786946347</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -34246,7 +34294,7 @@
       <c r="Z14" s="12"/>
     </row>
     <row r="15">
-      <c r="A15" s="14">
+      <c r="A15" s="13">
         <v>14.0</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -34270,8 +34318,8 @@
       <c r="H15" s="11">
         <v>75.0</v>
       </c>
-      <c r="I15" s="11">
-        <v>-2.36707820978742</v>
+      <c r="I15" s="19">
+        <v>72.6329217902126</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
@@ -34292,7 +34340,7 @@
       <c r="Z15" s="12"/>
     </row>
     <row r="16">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <v>15.0</v>
       </c>
       <c r="B16" s="16" t="s">
@@ -34316,8 +34364,8 @@
       <c r="H16" s="17">
         <v>140.0</v>
       </c>
-      <c r="I16" s="17">
-        <v>-20.3878527020564</v>
+      <c r="I16" s="20">
+        <v>119.612147297944</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>

</xml_diff>